<commit_message>
ready for linux bnk
</commit_message>
<xml_diff>
--- a/prediction accuracy.xlsx
+++ b/prediction accuracy.xlsx
@@ -93,10 +93,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,7 +409,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,22 +421,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -644,225 +644,225 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>83.954999999999998</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>99.466999999999999</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>79.968000000000004</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>88.674000000000007</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>84.188000000000002</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>89.24</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>83.622</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>99.977000000000004</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>72.728999999999999</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>84.320999999999998</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>83.498999999999995</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="1">
         <v>84.442999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>5</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>100</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>80.510999999999996</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>89.411000000000001</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>86.010999999999996</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>92.022000000000006</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>100</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>72.454999999999998</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>85.277000000000001</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <v>84.366</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <v>87.688000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>100</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>80.712999999999994</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>89.564999999999998</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>89.697999999999993</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>98.26</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>100</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>73.054000000000002</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>85.384</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <v>86.22</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="1">
         <v>94.593000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>50</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>100</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>80.650000000000006</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>89.91</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>92.805000000000007</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>100</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>100</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>73.052000000000007</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>85.634</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <v>89.606999999999999</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="1">
         <v>99.224999999999994</v>
       </c>
     </row>

</xml_diff>